<commit_message>
working http server routes and responses
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70BB81E-05EC-4ACA-9DC1-7C07FEDAF485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFDDF66-61E2-41E0-990D-294249555D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Data</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Abbozzo diagramma dei casi d'uso con inserimento delle descrizioni brevi e relazioni ipotetiche </t>
   </si>
   <si>
-    <t>Selezione di circa il 10% dei casi d'uso da dettagliare in base a priorità architeturale, elevato valore ai fini del funzionamento del progetto. (3 sui 28 identificait finora)</t>
-  </si>
-  <si>
     <t>Vengono dettagliati i 3 casi d'uso individuati</t>
   </si>
   <si>
@@ -117,6 +114,57 @@
   </si>
   <si>
     <t>caso d'uso inserisci comune</t>
+  </si>
+  <si>
+    <t>si inizia lo sviluppo dei casi d'uso "inserisci nuovo comune" "inserisci nuovo poi"</t>
+  </si>
+  <si>
+    <t>Selezione di circa il 15% dei casi d'uso da dettagliare in base a priorità architeturale, elevato valore ai fini del funzionamento del progetto. (4 sui 28 identificait finora)</t>
+  </si>
+  <si>
+    <t>Fine prima interazione</t>
+  </si>
+  <si>
+    <t>Avvio seconda iterazione</t>
+  </si>
+  <si>
+    <t>Si identificano altri 5 casi d'uso pari a circa il 15 % del totale e si provvede alla definizione della versione dettagliata</t>
+  </si>
+  <si>
+    <t>registrazione nuovo utente</t>
+  </si>
+  <si>
+    <t>autenticazione utente</t>
+  </si>
+  <si>
+    <t>assegna ruolo utente</t>
+  </si>
+  <si>
+    <t>aggiungi POI certificato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si inseriscono paragrafi descrittivi brevi su altri casi d'uso </t>
+  </si>
+  <si>
+    <t>richiedere inserimento nuovo comune</t>
+  </si>
+  <si>
+    <t>creare un contest di contribuzione</t>
+  </si>
+  <si>
+    <t>valida le proposte di Contest di contribuzione</t>
+  </si>
+  <si>
+    <t>valida POI</t>
+  </si>
+  <si>
+    <t>modifica dati comune</t>
+  </si>
+  <si>
+    <t>rimuovere comune</t>
+  </si>
+  <si>
+    <t>Si iniza la stesura del diagramma entità relazioni del database</t>
   </si>
 </sst>
 </file>
@@ -140,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +207,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -172,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -184,9 +244,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -521,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I29"/>
+  <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,15 +636,15 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
@@ -613,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -622,22 +692,22 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C13" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C13" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C14" s="6" t="s">
-        <v>14</v>
+      <c r="C14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -646,8 +716,8 @@
       <c r="B15" s="5">
         <v>1</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>17</v>
+      <c r="C15" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -658,10 +728,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" s="5">
         <v>1</v>
       </c>
@@ -669,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B18" s="5">
         <v>1</v>
       </c>
@@ -677,7 +747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45588</v>
       </c>
@@ -685,18 +755,18 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45589</v>
       </c>
@@ -704,54 +774,185 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B22" s="5">
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>26</v>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="9">
+        <v>45596</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>45601</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C39" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C40" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C41" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C42" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="5">
+        <v>2</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C46" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C47" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C48" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C49" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C50" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>45638</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C45:H45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Design pattern Factory per la creazione dei controllers
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C8402B-7894-4344-9EED-38B9B3106B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230778B3-26B0-4E7C-BBEE-79E58BCFA449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView minimized="1" xWindow="-23773" yWindow="4613" windowWidth="12813" windowHeight="6714" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Data</t>
   </si>
@@ -110,9 +110,6 @@
     <t>25/10/2024 al 31/102024</t>
   </si>
   <si>
-    <t>si inizia lo sviluppo dei casi d'uso "inserisci nuovo comune" "inserisci nuovo poi"</t>
-  </si>
-  <si>
     <t>Selezione di circa il 15% dei casi d'uso da dettagliare in base a priorità architeturale, elevato valore ai fini del funzionamento del progetto. (4 sui 28 identificait finora)</t>
   </si>
   <si>
@@ -134,30 +131,6 @@
     <t>assegna ruolo utente</t>
   </si>
   <si>
-    <t>aggiungi POI certificato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si inseriscono paragrafi descrittivi brevi su altri casi d'uso </t>
-  </si>
-  <si>
-    <t>richiedere inserimento nuovo comune</t>
-  </si>
-  <si>
-    <t>creare un contest di contribuzione</t>
-  </si>
-  <si>
-    <t>valida le proposte di Contest di contribuzione</t>
-  </si>
-  <si>
-    <t>valida POI</t>
-  </si>
-  <si>
-    <t>modifica dati comune</t>
-  </si>
-  <si>
-    <t>rimuovere comune</t>
-  </si>
-  <si>
     <t>Si iniza la stesura del diagramma entità relazioni del database</t>
   </si>
   <si>
@@ -171,6 +144,30 @@
   </si>
   <si>
     <t>3 inserisci geolocation</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>dettaglio poi</t>
+  </si>
+  <si>
+    <t>Registrazione nuovo utente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok </t>
+  </si>
+  <si>
+    <t xml:space="preserve">si inizia lo sviluppo dei casi d'uso "inserisci nuovo comune" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si inseriscono paragrafi descrittivi brevi su tutti i casi d'uso </t>
+  </si>
+  <si>
+    <t>valida contenuto</t>
+  </si>
+  <si>
+    <t>autocertificazione contento</t>
   </si>
 </sst>
 </file>
@@ -596,17 +593,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I52"/>
+  <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="25.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -688,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -798,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -818,7 +815,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C28" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -831,17 +828,17 @@
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -849,7 +846,7 @@
         <v>45596</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -863,7 +860,7 @@
         <v>45601</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -871,103 +868,88 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C38" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="7" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C40" s="7" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C41" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C44" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>45638</v>
+      </c>
       <c r="B45" s="5">
         <v>2</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C46" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C47" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C48" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C49" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C50" s="7" t="s">
+      <c r="C45" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
-        <v>45638</v>
-      </c>
-      <c r="B52" s="5">
-        <v>2</v>
-      </c>
-      <c r="C52" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="C38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementazione registrazione utente e autenticazione utente
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230778B3-26B0-4E7C-BBEE-79E58BCFA449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B3FD06-CBF2-402D-9244-402120FA8AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-23773" yWindow="4613" windowWidth="12813" windowHeight="6714" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Data</t>
   </si>
@@ -168,6 +168,30 @@
   </si>
   <si>
     <t>autocertificazione contento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sviluppo 4 casi d'uso </t>
+  </si>
+  <si>
+    <t>Autenticazione utente</t>
+  </si>
+  <si>
+    <t>Assegna ruolo utente</t>
+  </si>
+  <si>
+    <t>implementato</t>
+  </si>
+  <si>
+    <t>completato</t>
+  </si>
+  <si>
+    <t>Consultare dettaglio POI</t>
+  </si>
+  <si>
+    <t>dettagliato con diagrammi</t>
+  </si>
+  <si>
+    <t>da implementare</t>
   </si>
 </sst>
 </file>
@@ -235,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -259,6 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -593,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I45"/>
+  <dimension ref="A3:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,15 +855,24 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D29" s="13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="D30" s="13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -944,6 +978,55 @@
       </c>
       <c r="C45" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C47" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C48" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C49" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+      <c r="F50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+      <c r="F51" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementazione elimina utente e ottieni dettaglio utente
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B3FD06-CBF2-402D-9244-402120FA8AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F435D1FC-18F6-42D9-A140-EFF5317E605E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Data</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Assegna ruolo utente</t>
   </si>
   <si>
-    <t>implementato</t>
-  </si>
-  <si>
     <t>completato</t>
   </si>
   <si>
@@ -192,6 +189,33 @@
   </si>
   <si>
     <t>da implementare</t>
+  </si>
+  <si>
+    <t>dettagliato con diagramma</t>
+  </si>
+  <si>
+    <t>Validazione contenuti</t>
+  </si>
+  <si>
+    <t>Rimozione comune</t>
+  </si>
+  <si>
+    <t>dettagliato - da rivedere diagramma di sequenza</t>
+  </si>
+  <si>
+    <t>Visualizza dettaglio Comune</t>
+  </si>
+  <si>
+    <t>Ricerca Comune</t>
+  </si>
+  <si>
+    <t>Rimozione Utente</t>
+  </si>
+  <si>
+    <t>Si identificano altri 6 casi d'uso da dettagliare</t>
+  </si>
+  <si>
+    <t>Ottieni Dettaglio Utente</t>
   </si>
 </sst>
 </file>
@@ -215,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -259,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -277,13 +307,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -618,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I51"/>
+  <dimension ref="A3:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,15 +694,15 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
@@ -855,24 +886,24 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>48</v>
+      <c r="D29" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>48</v>
+      <c r="D30" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>48</v>
+      <c r="D31" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -912,14 +943,14 @@
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="7" t="s">
@@ -987,46 +1018,123 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C48" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
         <v>49</v>
       </c>
-      <c r="D48" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C49" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C50" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D50" t="s">
-        <v>51</v>
+      <c r="D50" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="F50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C51" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>45656</v>
+      </c>
+      <c r="B54" s="5">
+        <v>3</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C55" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" t="s">
         <v>51</v>
       </c>
-      <c r="F51" t="s">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" t="s">
         <v>50</v>
+      </c>
+      <c r="F56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring ed ottimizzazione delle classi di modello
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA13A77-AEDB-49FF-A78C-5DEB06EE054C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B17DEA-6F32-4CD4-A4FF-37AE368DDC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" activeTab="1" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>Data</t>
   </si>
@@ -255,10 +255,13 @@
     <t>poi</t>
   </si>
   <si>
-    <t>con geolocation e municipality</t>
-  </si>
-  <si>
     <t>ottienibyId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con geolocation </t>
+  </si>
+  <si>
+    <t>verificare</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +316,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -326,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -345,13 +354,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -688,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
   <dimension ref="A3:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60:G60"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,15 +741,15 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
@@ -980,14 +990,14 @@
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="7" t="s">
@@ -1001,7 +1011,7 @@
       <c r="C40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1009,7 +1019,7 @@
       <c r="C41" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1017,7 +1027,7 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1025,7 +1035,7 @@
       <c r="C43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1033,7 +1043,7 @@
       <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1148,7 +1158,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C58" t="s">
+      <c r="C58" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="11" t="s">
@@ -1193,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84958B76-6CF5-42BE-9F9D-47765C5E6CD8}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1209,23 +1219,23 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>67</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>71</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="14"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1261,13 +1271,13 @@
         <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -1276,6 +1286,15 @@
       </c>
       <c r="B6" t="s">
         <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
refactoring classi httprequesthandler e controllers
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B17DEA-6F32-4CD4-A4FF-37AE368DDC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD9334-7F95-4624-ACA8-600EF673408A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Data</t>
   </si>
@@ -138,9 +138,6 @@
     <t>inizio sviluppo dell'architettura dell' applicazione e primi casi d'uso senza SpringBoot</t>
   </si>
   <si>
-    <t>1 caso d'uso inserisci comune</t>
-  </si>
-  <si>
     <t>2 inserisci nuovo poi</t>
   </si>
   <si>
@@ -262,6 +259,33 @@
   </si>
   <si>
     <t>verificare</t>
+  </si>
+  <si>
+    <t>Si identificano 6 casi d'uso da dettagliare</t>
+  </si>
+  <si>
+    <t>Associa Poi</t>
+  </si>
+  <si>
+    <t>Inserisci nuova attività</t>
+  </si>
+  <si>
+    <t>Modifica Poi</t>
+  </si>
+  <si>
+    <t>Rimuovi Poi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifica Attività </t>
+  </si>
+  <si>
+    <t>Rimuovi Attività</t>
+  </si>
+  <si>
+    <t>Crea Nuovo Comune</t>
+  </si>
+  <si>
+    <t>Ricerca Poi</t>
   </si>
 </sst>
 </file>
@@ -355,13 +379,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -696,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I60"/>
+  <dimension ref="A3:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,15 +765,15 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
@@ -918,7 +942,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C28" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -931,26 +955,26 @@
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -980,71 +1004,71 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C41" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>36</v>
+      <c r="D42" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>36</v>
+      <c r="D43" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>36</v>
+      <c r="D44" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -1060,51 +1084,51 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C47" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
         <v>48</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C49" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C50" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="F51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -1115,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
@@ -1126,68 +1150,144 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C55" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56" t="s">
         <v>50</v>
-      </c>
-      <c r="F56" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" t="s">
         <v>53</v>
-      </c>
-      <c r="D57" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C58" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" t="s">
         <v>50</v>
-      </c>
-      <c r="F59" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C60" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F60" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>45663</v>
+      </c>
+      <c r="B63" s="5">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="F67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>80</v>
+      </c>
+      <c r="D69">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C72" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1196,6 +1296,7 @@
     <mergeCell ref="C38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1215,22 +1316,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="I3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1239,78 +1340,78 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring classi di gestione delle rotte e controllers
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD9334-7F95-4624-ACA8-600EF673408A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BB1866-9AB6-481C-BF78-6C7ED8CDCD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
   <si>
     <t>Data</t>
   </si>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
   <dimension ref="A3:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,6 +731,7 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="25.81640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1160,7 +1161,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C56" t="s">
+      <c r="C56" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D56" t="s">
@@ -1171,11 +1172,11 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C57" t="s">
+      <c r="C57" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F57" t="s">
         <v>53</v>
@@ -1193,11 +1194,11 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C59" t="s">
+      <c r="C59" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F59" t="s">
         <v>50</v>
@@ -1226,11 +1227,14 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C64" t="s">
+      <c r="C64" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="7">
         <v>1</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="F64" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
casi d'uso correlati alle activities - introduzione context per tracciamento utente autenticato
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BB1866-9AB6-481C-BF78-6C7ED8CDCD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0500D4-F7BE-4535-B147-E47EFBC936CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>Data</t>
   </si>
@@ -129,9 +129,6 @@
     <t>autenticazione utente</t>
   </si>
   <si>
-    <t>assegna ruolo utente</t>
-  </si>
-  <si>
     <t>Si iniza la stesura del diagramma entità relazioni del database</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
   </si>
   <si>
     <t>dettagliato con diagrammi</t>
-  </si>
-  <si>
-    <t>da implementare</t>
   </si>
   <si>
     <t>dettagliato con diagramma</t>
@@ -292,7 +286,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +298,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,7 +351,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -377,9 +386,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -722,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
   <dimension ref="A3:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,15 +777,15 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
@@ -923,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -943,7 +954,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C28" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -956,27 +967,33 @@
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
@@ -1005,72 +1022,80 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" t="s">
-        <v>35</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C40" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>38</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C41" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C43" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C44" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -1080,56 +1105,60 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C47" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C48" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C49" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C50" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C51" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -1140,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
@@ -1151,68 +1180,74 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C55" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C56" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D56" t="s">
         <v>49</v>
       </c>
-      <c r="F56" t="s">
-        <v>50</v>
+      <c r="D56" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C57" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D57" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C58" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C59" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C60" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -1223,59 +1258,65 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C64" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D64" s="7">
         <v>1</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C65" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65">
+      <c r="C65" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="13">
         <v>2</v>
       </c>
+      <c r="E65" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="F65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="F66" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C67" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67">
+      <c r="C67" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="13">
         <v>4</v>
       </c>
+      <c r="E67" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="F67" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D68">
         <v>5</v>
@@ -1283,7 +1324,7 @@
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D69">
         <v>6</v>
@@ -1291,7 +1332,7 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1320,102 +1361,102 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>59</v>
+      <c r="A3" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="D3" s="12" t="s">
-        <v>66</v>
+      <c r="D3" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="12" t="s">
-        <v>70</v>
+      <c r="I3" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="12"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
         <v>69</v>
       </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
         <v>71</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casi uso modifica comune segnala contenuto quarta iterazione
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0500D4-F7BE-4535-B147-E47EFBC936CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26417FD6-A6F8-45B0-AEC0-1E7B957C7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
+    <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>Data</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>Ricerca Poi</t>
+  </si>
+  <si>
+    <t>Segnala contenuto</t>
+  </si>
+  <si>
+    <t>Modifica Comune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dettaglio con diagramma </t>
+  </si>
+  <si>
+    <t>Modifica dati Utente</t>
+  </si>
+  <si>
+    <t>Salva informazioni per visite future</t>
   </si>
 </sst>
 </file>
@@ -731,17 +746,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I72"/>
+  <dimension ref="A3:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="25.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
     <col min="5" max="5" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1275,7 +1290,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C65" s="13" t="s">
         <v>80</v>
       </c>
@@ -1289,18 +1304,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C66" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C66" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="13">
         <v>3</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="F66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C67" s="13" t="s">
         <v>76</v>
       </c>
@@ -1314,25 +1332,75 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C68" t="s">
-        <v>77</v>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C68" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="D68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C69" t="s">
-        <v>78</v>
+      <c r="F68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C69" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="D69">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="F69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>45703</v>
+      </c>
+      <c r="B72" s="5">
+        <v>5</v>
+      </c>
       <c r="C72" t="s">
         <v>73</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C75" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" s="13">
+        <v>4</v>
+      </c>
+      <c r="F75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completamento casi d'uso modifica comune e modifica geolocations
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26417FD6-A6F8-45B0-AEC0-1E7B957C7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5ECD42-8AB4-4CC8-A7C0-C4DEF8EA3485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Data</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>Salva informazioni per visite future</t>
+  </si>
+  <si>
+    <t>dettaglio con diagramma</t>
+  </si>
+  <si>
+    <t>dettaglio</t>
   </si>
 </sst>
 </file>
@@ -749,7 +755,7 @@
   <dimension ref="A3:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,19 +1367,25 @@
       <c r="B72" s="5">
         <v>5</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="13" t="s">
         <v>73</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
+      <c r="F72" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C73" t="s">
+      <c r="C73" s="13" t="s">
         <v>77</v>
       </c>
       <c r="D73">
         <v>2</v>
+      </c>
+      <c r="F73" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -1382,6 +1394,9 @@
       </c>
       <c r="D74">
         <v>3</v>
+      </c>
+      <c r="F74" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
implementazione caso segnalazione contenuto / poi
</commit_message>
<xml_diff>
--- a/docs/log-iterazioni.xlsx
+++ b/docs/log-iterazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\PoiFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5ECD42-8AB4-4CC8-A7C0-C4DEF8EA3485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807A9174-9F2B-42CC-9391-D4FCC03A56BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="2220" windowWidth="25786" windowHeight="13987" xr2:uid="{B497E548-47E7-4AE8-B3C5-B4CDBDB7A71F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>Data</t>
   </si>
@@ -300,7 +300,7 @@
     <t>dettaglio con diagramma</t>
   </si>
   <si>
-    <t>dettaglio</t>
+    <t>Richiedi adesione Contest</t>
   </si>
 </sst>
 </file>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0CD4DD-D721-47BE-98D0-EA30A7BAA41A}">
-  <dimension ref="A3:I76"/>
+  <dimension ref="A3:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D65" s="13">
@@ -1311,7 +1311,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D66" s="13">
@@ -1325,7 +1325,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="13">
@@ -1339,7 +1339,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D68">
@@ -1350,11 +1350,14 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="13">
         <v>6</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="F69" t="s">
         <v>83</v>
@@ -1367,7 +1370,7 @@
       <c r="B72" s="5">
         <v>5</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D72">
@@ -1378,7 +1381,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D73">
@@ -1389,18 +1392,18 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C74" t="s">
+      <c r="C74" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D74">
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D75" s="13">
@@ -1411,11 +1414,25 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C76" t="s">
+      <c r="C76" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D76">
         <v>5</v>
+      </c>
+      <c r="F76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C77" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77">
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>